<commit_message>
Added hadeling of Halv Produkt vid enbart växelvis adress
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon27san\Documents\UiPath\Skapa Reskort\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Jonas\RPA-Skapa_Reskort\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>LatestRun_SkapaReskort_Grundskola</t>
+  </si>
+  <si>
+    <t>HalvProdukt</t>
+  </si>
+  <si>
+    <t>Ja</t>
   </si>
 </sst>
 </file>
@@ -560,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -639,7 +645,14 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2805,7 +2818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated to make different lists depeding if you want only students that travel within the kommun or within the län to different kommuns than sundsvall
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -173,12 +173,6 @@
     <t>Grundskola_ExcelFilePath</t>
   </si>
   <si>
-    <t>Skolportalen_Mall</t>
-  </si>
-  <si>
-    <t>Filsökväg_För_Elevresor</t>
-  </si>
-  <si>
     <t>LatestRun_SkapaReskort_Grundskola</t>
   </si>
   <si>
@@ -186,6 +180,21 @@
   </si>
   <si>
     <t>Ja</t>
+  </si>
+  <si>
+    <t>Skolportalen_Template</t>
+  </si>
+  <si>
+    <t>FilePath_Elevresor</t>
+  </si>
+  <si>
+    <t>Conversionfile_Elevresor</t>
+  </si>
+  <si>
+    <t>ConversionExcelFilepath</t>
+  </si>
+  <si>
+    <t>FilePath_Grundskola</t>
   </si>
 </sst>
 </file>
@@ -564,7 +573,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -644,10 +653,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1652,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2812,7 +2821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2870,10 +2879,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2897,26 +2906,33 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Replace " " with "" for zipcode
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -164,15 +164,6 @@
     <t>LatestRun_SkapaReskort_Elevresor</t>
   </si>
   <si>
-    <t>ExcelFilePath</t>
-  </si>
-  <si>
-    <t>Elevresor_ExcelFilePath</t>
-  </si>
-  <si>
-    <t>Grundskola_ExcelFilePath</t>
-  </si>
-  <si>
     <t>LatestRun_SkapaReskort_Grundskola</t>
   </si>
   <si>
@@ -195,6 +186,12 @@
   </si>
   <si>
     <t>FilePath_Grundskola</t>
+  </si>
+  <si>
+    <t>FilePath_Masterfile_Elevresor</t>
+  </si>
+  <si>
+    <t>FilePath_Masterfile_Grundskola</t>
   </si>
 </sst>
 </file>
@@ -653,10 +650,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2819,10 +2816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2879,10 +2876,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2895,26 +2892,26 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2927,13 +2924,20 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3924,6 +3928,7 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Deleted some unnecessarily logic for a old solution.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -159,12 +159,6 @@
   </si>
   <si>
     <t>Environment</t>
-  </si>
-  <si>
-    <t>LatestRun_SkapaReskort_Elevresor</t>
-  </si>
-  <si>
-    <t>LatestRun_SkapaReskort_Grundskola</t>
   </si>
   <si>
     <t>HalvProdukt</t>
@@ -650,10 +644,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2816,10 +2810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2876,68 +2870,54 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3927,8 +3907,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>